<commit_message>
Remove JSON key file from Git tracking
</commit_message>
<xml_diff>
--- a/app/src/main/assets/daily_word.xlsx
+++ b/app/src/main/assets/daily_word.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00_spa_study_app\app\src\main\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spa_study_app\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB47598-660D-49AE-A4C2-DC5ABFD97675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CC1096-D794-4617-B704-BCB43C828FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67170" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4263B891-630D-40DF-9C1A-1DC01B50E521}"/>
+    <workbookView xWindow="6760" yWindow="940" windowWidth="20780" windowHeight="20040" xr2:uid="{4263B891-630D-40DF-9C1A-1DC01B50E521}"/>
   </bookViews>
   <sheets>
     <sheet name="word 예시" sheetId="1" r:id="rId1"/>
@@ -1308,15 +1308,15 @@
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="36.25" customWidth="1"/>
     <col min="2" max="2" width="18.58203125" customWidth="1"/>
-    <col min="3" max="3" width="66.9140625" customWidth="1"/>
-    <col min="4" max="4" width="71.25" customWidth="1"/>
+    <col min="3" max="3" width="71.25" customWidth="1"/>
+    <col min="4" max="4" width="66.9140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
@@ -1327,10 +1327,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -1341,10 +1341,10 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -1355,10 +1355,10 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -1369,10 +1369,10 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -1383,10 +1383,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -1397,10 +1397,10 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -1411,10 +1411,10 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
         <v>52</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -1439,10 +1439,10 @@
         <v>32</v>
       </c>
       <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
         <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -1453,10 +1453,10 @@
         <v>36</v>
       </c>
       <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
         <v>101</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -1467,10 +1467,10 @@
         <v>37</v>
       </c>
       <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
         <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -1481,10 +1481,10 @@
         <v>38</v>
       </c>
       <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
         <v>39</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
@@ -1495,10 +1495,10 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -1509,10 +1509,10 @@
         <v>42</v>
       </c>
       <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
         <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
@@ -1523,10 +1523,10 @@
         <v>47</v>
       </c>
       <c r="C15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" t="s">
         <v>99</v>
-      </c>
-      <c r="D15" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
@@ -1537,10 +1537,10 @@
         <v>48</v>
       </c>
       <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
         <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
@@ -1551,10 +1551,10 @@
         <v>53</v>
       </c>
       <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
         <v>55</v>
-      </c>
-      <c r="D17" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
@@ -1565,10 +1565,10 @@
         <v>57</v>
       </c>
       <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
         <v>59</v>
-      </c>
-      <c r="D18" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
@@ -1579,10 +1579,10 @@
         <v>61</v>
       </c>
       <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
         <v>63</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
@@ -1621,10 +1621,10 @@
         <v>68</v>
       </c>
       <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
         <v>70</v>
-      </c>
-      <c r="D22" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
@@ -1635,10 +1635,10 @@
         <v>72</v>
       </c>
       <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
         <v>74</v>
-      </c>
-      <c r="D23" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
@@ -1649,10 +1649,10 @@
         <v>76</v>
       </c>
       <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" t="s">
         <v>78</v>
-      </c>
-      <c r="D24" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
@@ -1663,10 +1663,10 @@
         <v>80</v>
       </c>
       <c r="C25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" t="s">
         <v>96</v>
-      </c>
-      <c r="D25" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
@@ -1677,10 +1677,10 @@
         <v>81</v>
       </c>
       <c r="C26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" t="s">
         <v>94</v>
-      </c>
-      <c r="D26" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
@@ -1691,10 +1691,10 @@
         <v>83</v>
       </c>
       <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" t="s">
         <v>90</v>
-      </c>
-      <c r="D27" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
@@ -1705,10 +1705,10 @@
         <v>85</v>
       </c>
       <c r="C28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" t="s">
         <v>88</v>
-      </c>
-      <c r="D28" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
@@ -1719,10 +1719,10 @@
         <v>86</v>
       </c>
       <c r="C29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" t="s">
         <v>92</v>
-      </c>
-      <c r="D29" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
@@ -1733,10 +1733,10 @@
         <v>102</v>
       </c>
       <c r="C30" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" t="s">
         <v>108</v>
-      </c>
-      <c r="D30" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
@@ -1747,10 +1747,10 @@
         <v>104</v>
       </c>
       <c r="C31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" t="s">
         <v>106</v>
-      </c>
-      <c r="D31" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
@@ -1761,10 +1761,10 @@
         <v>110</v>
       </c>
       <c r="C32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" t="s">
         <v>112</v>
-      </c>
-      <c r="D32" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
@@ -1775,10 +1775,10 @@
         <v>114</v>
       </c>
       <c r="C33" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" t="s">
         <v>116</v>
-      </c>
-      <c r="D33" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
@@ -1789,10 +1789,10 @@
         <v>118</v>
       </c>
       <c r="C34" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" t="s">
         <v>119</v>
-      </c>
-      <c r="D34" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
@@ -1803,10 +1803,10 @@
         <v>121</v>
       </c>
       <c r="C35" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" t="s">
         <v>123</v>
-      </c>
-      <c r="D35" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
@@ -1817,10 +1817,10 @@
         <v>125</v>
       </c>
       <c r="C36" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" t="s">
         <v>134</v>
-      </c>
-      <c r="D36" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
@@ -1831,10 +1831,10 @@
         <v>132</v>
       </c>
       <c r="C37" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" t="s">
         <v>136</v>
-      </c>
-      <c r="D37" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
@@ -1845,10 +1845,10 @@
         <v>138</v>
       </c>
       <c r="C38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" t="s">
         <v>140</v>
-      </c>
-      <c r="D38" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
@@ -1859,10 +1859,10 @@
         <v>142</v>
       </c>
       <c r="C39" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" t="s">
         <v>144</v>
-      </c>
-      <c r="D39" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
@@ -1873,10 +1873,10 @@
         <v>146</v>
       </c>
       <c r="C40" t="s">
+        <v>149</v>
+      </c>
+      <c r="D40" t="s">
         <v>148</v>
-      </c>
-      <c r="D40" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
@@ -1887,10 +1887,10 @@
         <v>150</v>
       </c>
       <c r="C41" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41" t="s">
         <v>152</v>
-      </c>
-      <c r="D41" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
@@ -1901,10 +1901,10 @@
         <v>154</v>
       </c>
       <c r="C42" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42" t="s">
         <v>156</v>
-      </c>
-      <c r="D42" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
@@ -1915,10 +1915,10 @@
         <v>158</v>
       </c>
       <c r="C43" t="s">
+        <v>161</v>
+      </c>
+      <c r="D43" t="s">
         <v>160</v>
-      </c>
-      <c r="D43" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
@@ -1929,10 +1929,10 @@
         <v>162</v>
       </c>
       <c r="C44" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" t="s">
         <v>166</v>
-      </c>
-      <c r="D44" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
@@ -1943,10 +1943,10 @@
         <v>163</v>
       </c>
       <c r="C45" t="s">
+        <v>169</v>
+      </c>
+      <c r="D45" t="s">
         <v>168</v>
-      </c>
-      <c r="D45" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
@@ -1957,10 +1957,10 @@
         <v>170</v>
       </c>
       <c r="C46" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46" t="s">
         <v>172</v>
-      </c>
-      <c r="D46" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
@@ -1971,10 +1971,10 @@
         <v>174</v>
       </c>
       <c r="C47" t="s">
+        <v>177</v>
+      </c>
+      <c r="D47" t="s">
         <v>176</v>
-      </c>
-      <c r="D47" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
@@ -1985,10 +1985,10 @@
         <v>178</v>
       </c>
       <c r="C48" t="s">
+        <v>181</v>
+      </c>
+      <c r="D48" t="s">
         <v>180</v>
-      </c>
-      <c r="D48" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
@@ -1999,10 +1999,10 @@
         <v>182</v>
       </c>
       <c r="C49" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" t="s">
         <v>184</v>
-      </c>
-      <c r="D49" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
@@ -2013,10 +2013,10 @@
         <v>186</v>
       </c>
       <c r="C50" t="s">
+        <v>189</v>
+      </c>
+      <c r="D50" t="s">
         <v>188</v>
-      </c>
-      <c r="D50" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
@@ -2027,10 +2027,10 @@
         <v>190</v>
       </c>
       <c r="C51" t="s">
+        <v>193</v>
+      </c>
+      <c r="D51" t="s">
         <v>192</v>
-      </c>
-      <c r="D51" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
@@ -2041,10 +2041,10 @@
         <v>194</v>
       </c>
       <c r="C52" t="s">
+        <v>197</v>
+      </c>
+      <c r="D52" t="s">
         <v>196</v>
-      </c>
-      <c r="D52" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
@@ -2055,10 +2055,10 @@
         <v>198</v>
       </c>
       <c r="C53" t="s">
+        <v>213</v>
+      </c>
+      <c r="D53" t="s">
         <v>212</v>
-      </c>
-      <c r="D53" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
@@ -2069,10 +2069,10 @@
         <v>200</v>
       </c>
       <c r="C54" t="s">
+        <v>215</v>
+      </c>
+      <c r="D54" t="s">
         <v>214</v>
-      </c>
-      <c r="D54" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
@@ -2083,10 +2083,10 @@
         <v>202</v>
       </c>
       <c r="C55" t="s">
+        <v>217</v>
+      </c>
+      <c r="D55" t="s">
         <v>216</v>
-      </c>
-      <c r="D55" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
@@ -2097,10 +2097,10 @@
         <v>204</v>
       </c>
       <c r="C56" t="s">
+        <v>219</v>
+      </c>
+      <c r="D56" t="s">
         <v>218</v>
-      </c>
-      <c r="D56" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
@@ -2111,10 +2111,10 @@
         <v>206</v>
       </c>
       <c r="C57" t="s">
+        <v>221</v>
+      </c>
+      <c r="D57" t="s">
         <v>220</v>
-      </c>
-      <c r="D57" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
@@ -2125,10 +2125,10 @@
         <v>207</v>
       </c>
       <c r="C58" t="s">
+        <v>223</v>
+      </c>
+      <c r="D58" t="s">
         <v>222</v>
-      </c>
-      <c r="D58" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
@@ -2139,10 +2139,10 @@
         <v>208</v>
       </c>
       <c r="C59" t="s">
+        <v>225</v>
+      </c>
+      <c r="D59" t="s">
         <v>224</v>
-      </c>
-      <c r="D59" t="s">
-        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>